<commit_message>
Adicionando minhas imagens no formato de dataframes contendo string em base64
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AriosvaldoBarros\Desktop\Projeto final - Aprendizado de Máquina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BFA73DF-BAD5-4642-81A9-4F1268152934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9401B79B-A3FC-4CE2-8BE7-9198C7C14E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5910" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{1AF00C1C-39EC-4648-B1B0-894BAF27F7E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{1AF00C1C-39EC-4648-B1B0-894BAF27F7E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -216,9 +216,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -228,7 +225,7 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -237,13 +234,14 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1578,22 +1576,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -1713,40 +1711,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1760,17 +1758,17 @@
       <c r="C4" s="2">
         <v>1000</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="8">
-        <v>45</v>
-      </c>
-      <c r="F4" s="7">
+      <c r="E4" s="7">
+        <v>45</v>
+      </c>
+      <c r="F4" s="6">
         <v>0.55630000000000002</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="6">
+      <c r="G4" s="6"/>
+      <c r="H4" s="5">
         <v>22.27</v>
       </c>
     </row>
@@ -1785,22 +1783,22 @@
         <f>C4</f>
         <v>1000</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <f>D4+1</f>
         <v>2</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <f>E4</f>
         <v>45</v>
       </c>
       <c r="F5" s="2">
         <v>0.29709999999999998</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <f>IF(F5&lt;&gt;"",(F4-F5)/F4,"")</f>
         <v>0.46593564623404643</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <f>H4</f>
         <v>22.27</v>
       </c>
@@ -1816,22 +1814,22 @@
         <f t="shared" ref="C6:C14" si="0">C5</f>
         <v>1000</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <f t="shared" ref="D6:D18" si="1">D5+1</f>
         <v>3</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <f t="shared" ref="E6:E11" si="2">E5</f>
         <v>45</v>
       </c>
       <c r="F6" s="2">
         <v>0.1623</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <f t="shared" ref="G6:G48" si="3">IF(F6&lt;&gt;"",(F5-F6)/F5,"")</f>
         <v>0.45371928643554355</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <f t="shared" ref="H6:H28" si="4">H5</f>
         <v>22.27</v>
       </c>
@@ -1847,22 +1845,22 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="F7" s="2">
         <v>0.11650000000000001</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <f t="shared" si="3"/>
         <v>0.28219346888478125</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -1878,22 +1876,22 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="F8" s="2">
         <v>9.4399999999999998E-2</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <f t="shared" si="3"/>
         <v>0.18969957081545072</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -1909,22 +1907,22 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="F9" s="2">
         <v>8.1900000000000001E-2</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <f t="shared" si="3"/>
         <v>0.13241525423728812</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -1940,22 +1938,22 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="F10" s="2">
         <v>7.1499999999999994E-2</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <f t="shared" si="3"/>
         <v>0.12698412698412706</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -1971,22 +1969,22 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="F11" s="2">
         <v>7.0300000000000001E-2</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <f t="shared" si="3"/>
         <v>1.6783216783216683E-2</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2002,22 +2000,22 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <f>E11</f>
         <v>45</v>
       </c>
       <c r="F12" s="2">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <f t="shared" si="3"/>
         <v>4.6941678520625849E-2</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2033,22 +2031,22 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <f t="shared" ref="E13:E16" si="5">E12</f>
         <v>45</v>
       </c>
       <c r="F13" s="2">
         <v>6.2300000000000001E-2</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <f t="shared" si="3"/>
         <v>7.0149253731343328E-2</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2064,22 +2062,22 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="7">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="F14" s="2">
         <v>6.1400000000000003E-2</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
         <f t="shared" si="3"/>
         <v>1.4446227929373964E-2</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2095,22 +2093,22 @@
         <f t="shared" ref="C15:C18" si="6">C14</f>
         <v>1000</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="7">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="F15" s="2">
         <v>6.08E-2</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <f t="shared" si="3"/>
         <v>9.771986970684092E-3</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2126,22 +2124,22 @@
         <f t="shared" si="6"/>
         <v>1000</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="F16" s="2">
         <v>5.67E-2</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="8">
         <f t="shared" si="3"/>
         <v>6.7434210526315777E-2</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2157,22 +2155,22 @@
         <f t="shared" si="6"/>
         <v>1000</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <f t="shared" ref="E17:E18" si="7">E16</f>
         <v>45</v>
       </c>
       <c r="F17" s="2">
         <v>5.6500000000000002E-2</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="8">
         <f t="shared" si="3"/>
         <v>3.5273368606701726E-3</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2188,22 +2186,22 @@
         <f t="shared" si="6"/>
         <v>1000</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <f t="shared" si="7"/>
         <v>45</v>
       </c>
       <c r="F18" s="2">
         <v>5.0500000000000003E-2</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="8">
         <f t="shared" si="3"/>
         <v>0.1061946902654867</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2219,22 +2217,22 @@
         <f t="shared" ref="C19:C28" si="8">C18</f>
         <v>1000</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="7">
         <f t="shared" ref="D19:D28" si="9">D18+1</f>
         <v>16</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <f t="shared" ref="E19:E28" si="10">E18</f>
         <v>45</v>
       </c>
       <c r="F19" s="2">
         <v>0.37580000000000002</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="8">
         <f t="shared" si="3"/>
         <v>-6.441584158415842</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2250,22 +2248,22 @@
         <f t="shared" si="8"/>
         <v>1000</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="7">
         <f t="shared" si="9"/>
         <v>17</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="F20" s="2">
         <v>0.22259999999999999</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="8">
         <f t="shared" si="3"/>
         <v>0.40766365087812673</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2281,22 +2279,22 @@
         <f t="shared" si="8"/>
         <v>1000</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="7">
         <f t="shared" si="9"/>
         <v>18</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="7">
         <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="F21" s="2">
         <v>0.14460000000000001</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="8">
         <f t="shared" si="3"/>
         <v>0.35040431266846356</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2312,22 +2310,22 @@
         <f t="shared" si="8"/>
         <v>1000</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="7">
         <f t="shared" si="9"/>
         <v>19</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="7">
         <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="F22" s="2">
         <v>0.1231</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="8">
         <f t="shared" si="3"/>
         <v>0.14868603042876904</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2343,22 +2341,22 @@
         <f t="shared" si="8"/>
         <v>1000</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="7">
         <f t="shared" si="9"/>
         <v>20</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="F23" s="2">
         <v>9.7699999999999995E-2</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="8">
         <f t="shared" si="3"/>
         <v>0.206336311941511</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2374,22 +2372,22 @@
         <f t="shared" si="8"/>
         <v>1000</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="7">
         <f t="shared" si="9"/>
         <v>21</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="7">
         <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="F24" s="2">
         <v>8.5599999999999996E-2</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="8">
         <f t="shared" si="3"/>
         <v>0.12384851586489252</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2405,22 +2403,22 @@
         <f t="shared" si="8"/>
         <v>1000</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="7">
         <f t="shared" si="9"/>
         <v>22</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="7">
         <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="F25" s="2">
         <v>8.0199999999999994E-2</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="8">
         <f t="shared" si="3"/>
         <v>6.3084112149532731E-2</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2436,22 +2434,22 @@
         <f t="shared" si="8"/>
         <v>1000</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="7">
         <f t="shared" si="9"/>
         <v>23</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="7">
         <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="F26" s="2">
         <v>7.0699999999999999E-2</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="8">
         <f t="shared" si="3"/>
         <v>0.11845386533665829</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2467,22 +2465,22 @@
         <f t="shared" si="8"/>
         <v>1000</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="7">
         <f t="shared" si="9"/>
         <v>24</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="7">
         <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="F27" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="8">
         <f t="shared" si="3"/>
         <v>9.4766619519094736E-2</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2498,22 +2496,22 @@
         <f t="shared" si="8"/>
         <v>1000</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="7">
         <f t="shared" si="9"/>
         <v>25</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="7">
         <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="F28" s="2">
         <v>5.9799999999999999E-2</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="8">
         <f t="shared" si="3"/>
         <v>6.5625000000000031E-2</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="5">
         <f t="shared" si="4"/>
         <v>22.27</v>
       </c>
@@ -2529,22 +2527,22 @@
         <f t="shared" ref="C29:C37" si="11">C28</f>
         <v>1000</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="7">
         <f t="shared" ref="D29:D37" si="12">D28+1</f>
         <v>26</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="7">
         <f t="shared" ref="E29:E37" si="13">E28</f>
         <v>45</v>
       </c>
       <c r="F29" s="2">
         <v>5.2400000000000002E-2</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="8">
         <f t="shared" si="3"/>
         <v>0.12374581939799326</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="5">
         <f t="shared" ref="H29:H37" si="14">H28</f>
         <v>22.27</v>
       </c>
@@ -2560,22 +2558,22 @@
         <f t="shared" si="11"/>
         <v>1000</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="7">
         <f t="shared" si="12"/>
         <v>27</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="7">
         <f t="shared" si="13"/>
         <v>45</v>
       </c>
       <c r="F30" s="2">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="8">
         <f t="shared" si="3"/>
         <v>2.67175572519085E-2</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="5">
         <f t="shared" si="14"/>
         <v>22.27</v>
       </c>
@@ -2591,22 +2589,22 @@
         <f t="shared" si="11"/>
         <v>1000</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="7">
         <f t="shared" si="12"/>
         <v>28</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="7">
         <f t="shared" si="13"/>
         <v>45</v>
       </c>
       <c r="F31" s="2">
         <v>5.1299999999999998E-2</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="8">
         <f t="shared" si="3"/>
         <v>-5.8823529411765035E-3</v>
       </c>
-      <c r="H31" s="6">
+      <c r="H31" s="5">
         <f t="shared" si="14"/>
         <v>22.27</v>
       </c>
@@ -2622,22 +2620,22 @@
         <f t="shared" si="11"/>
         <v>1000</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="7">
         <f t="shared" si="12"/>
         <v>29</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="7">
         <f t="shared" si="13"/>
         <v>45</v>
       </c>
       <c r="F32" s="2">
         <v>4.8500000000000001E-2</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="8">
         <f t="shared" si="3"/>
         <v>5.4580896686159786E-2</v>
       </c>
-      <c r="H32" s="6">
+      <c r="H32" s="5">
         <f t="shared" si="14"/>
         <v>22.27</v>
       </c>
@@ -2653,22 +2651,22 @@
         <f t="shared" si="11"/>
         <v>1000</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="7">
         <f t="shared" si="12"/>
         <v>30</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="7">
         <f t="shared" si="13"/>
         <v>45</v>
       </c>
       <c r="F33" s="2">
         <v>4.6800000000000001E-2</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="8">
         <f t="shared" si="3"/>
         <v>3.5051546391752578E-2</v>
       </c>
-      <c r="H33" s="6">
+      <c r="H33" s="5">
         <f t="shared" si="14"/>
         <v>22.27</v>
       </c>
@@ -2684,22 +2682,22 @@
         <f t="shared" si="11"/>
         <v>1000</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="7">
         <f t="shared" si="12"/>
         <v>31</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="7">
         <f t="shared" si="13"/>
         <v>45</v>
       </c>
       <c r="F34" s="2">
         <v>4.5400000000000003E-2</v>
       </c>
-      <c r="G34" s="9">
+      <c r="G34" s="8">
         <f t="shared" si="3"/>
         <v>2.9914529914529881E-2</v>
       </c>
-      <c r="H34" s="6">
+      <c r="H34" s="5">
         <f t="shared" si="14"/>
         <v>22.27</v>
       </c>
@@ -2715,22 +2713,22 @@
         <f t="shared" si="11"/>
         <v>1000</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="7">
         <f t="shared" si="12"/>
         <v>32</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="7">
         <f t="shared" si="13"/>
         <v>45</v>
       </c>
       <c r="F35" s="2">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="8">
         <f t="shared" si="3"/>
         <v>5.7268722466960457E-2</v>
       </c>
-      <c r="H35" s="6">
+      <c r="H35" s="5">
         <f t="shared" si="14"/>
         <v>22.27</v>
       </c>
@@ -2746,22 +2744,22 @@
         <f t="shared" si="11"/>
         <v>1000</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D36" s="7">
         <f t="shared" si="12"/>
         <v>33</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="7">
         <f t="shared" si="13"/>
         <v>45</v>
       </c>
       <c r="F36" s="2">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="8">
         <f t="shared" si="3"/>
         <v>1.8691588785046617E-2</v>
       </c>
-      <c r="H36" s="6">
+      <c r="H36" s="5">
         <f t="shared" si="14"/>
         <v>22.27</v>
       </c>
@@ -2777,22 +2775,22 @@
         <f t="shared" si="11"/>
         <v>1000</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="7">
         <f t="shared" si="12"/>
         <v>34</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="7">
         <f t="shared" si="13"/>
         <v>45</v>
       </c>
       <c r="F37" s="2">
         <v>4.1799999999999997E-2</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="8">
         <f t="shared" si="3"/>
         <v>4.7619047619048976E-3</v>
       </c>
-      <c r="H37" s="6">
+      <c r="H37" s="5">
         <f t="shared" si="14"/>
         <v>22.27</v>
       </c>
@@ -2808,22 +2806,22 @@
         <f t="shared" ref="C38:C39" si="15">C37</f>
         <v>1000</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D38" s="7">
         <f t="shared" ref="D38:D39" si="16">D37+1</f>
         <v>35</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="7">
         <f t="shared" ref="E38:E39" si="17">E37</f>
         <v>45</v>
       </c>
       <c r="F38" s="2">
         <v>3.95E-2</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="8">
         <f t="shared" si="3"/>
         <v>5.5023923444975996E-2</v>
       </c>
-      <c r="H38" s="6">
+      <c r="H38" s="5">
         <f t="shared" ref="H38:H39" si="18">H37</f>
         <v>22.27</v>
       </c>
@@ -2839,22 +2837,22 @@
         <f t="shared" si="15"/>
         <v>1000</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D39" s="7">
         <f t="shared" si="16"/>
         <v>36</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="7">
         <f t="shared" si="17"/>
         <v>45</v>
       </c>
       <c r="F39" s="2">
         <v>4.02E-2</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="8">
         <f t="shared" si="3"/>
         <v>-1.7721518987341752E-2</v>
       </c>
-      <c r="H39" s="6">
+      <c r="H39" s="5">
         <f t="shared" si="18"/>
         <v>22.27</v>
       </c>
@@ -2870,22 +2868,22 @@
         <f t="shared" ref="C40:C41" si="19">C39</f>
         <v>1000</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D40" s="7">
         <f t="shared" ref="D40:D41" si="20">D39+1</f>
         <v>37</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E40" s="7">
         <f t="shared" ref="E40:E41" si="21">E39</f>
         <v>45</v>
       </c>
       <c r="F40" s="2">
         <v>3.8600000000000002E-2</v>
       </c>
-      <c r="G40" s="9">
+      <c r="G40" s="8">
         <f t="shared" si="3"/>
         <v>3.9800995024875552E-2</v>
       </c>
-      <c r="H40" s="6">
+      <c r="H40" s="5">
         <f t="shared" ref="H40:H41" si="22">H39</f>
         <v>22.27</v>
       </c>
@@ -2901,22 +2899,22 @@
         <f t="shared" si="19"/>
         <v>1000</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D41" s="7">
         <f t="shared" si="20"/>
         <v>38</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E41" s="7">
         <f t="shared" si="21"/>
         <v>45</v>
       </c>
       <c r="F41" s="2">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G41" s="9">
+      <c r="G41" s="8">
         <f t="shared" si="3"/>
         <v>6.7357512953368004E-2</v>
       </c>
-      <c r="H41" s="6">
+      <c r="H41" s="5">
         <f t="shared" si="22"/>
         <v>22.27</v>
       </c>
@@ -2932,22 +2930,22 @@
         <f t="shared" ref="C42:C43" si="23">C41</f>
         <v>1000</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D42" s="7">
         <f t="shared" ref="D42:D43" si="24">D41+1</f>
         <v>39</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E42" s="7">
         <f t="shared" ref="E42:E43" si="25">E41</f>
         <v>45</v>
       </c>
       <c r="F42" s="2">
         <v>3.5900000000000001E-2</v>
       </c>
-      <c r="G42" s="9">
+      <c r="G42" s="8">
         <f t="shared" si="3"/>
         <v>2.7777777777776647E-3</v>
       </c>
-      <c r="H42" s="6">
+      <c r="H42" s="5">
         <f t="shared" ref="H42:H43" si="26">H41</f>
         <v>22.27</v>
       </c>
@@ -2963,22 +2961,22 @@
         <f t="shared" si="23"/>
         <v>1000</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D43" s="7">
         <f t="shared" si="24"/>
         <v>40</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E43" s="7">
         <f t="shared" si="25"/>
         <v>45</v>
       </c>
       <c r="F43" s="2">
         <v>3.4099999999999998E-2</v>
       </c>
-      <c r="G43" s="9">
+      <c r="G43" s="8">
         <f t="shared" si="3"/>
         <v>5.0139275766016796E-2</v>
       </c>
-      <c r="H43" s="6">
+      <c r="H43" s="5">
         <f t="shared" si="26"/>
         <v>22.27</v>
       </c>
@@ -2994,22 +2992,22 @@
         <f t="shared" ref="C44:C47" si="27">C43</f>
         <v>1000</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D44" s="7">
         <f t="shared" ref="D44:D47" si="28">D43+1</f>
         <v>41</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E44" s="7">
         <f t="shared" ref="E44:E47" si="29">E43</f>
         <v>45</v>
       </c>
       <c r="F44" s="2">
         <v>3.27E-2</v>
       </c>
-      <c r="G44" s="9">
+      <c r="G44" s="8">
         <f t="shared" si="3"/>
         <v>4.105571847507327E-2</v>
       </c>
-      <c r="H44" s="6">
+      <c r="H44" s="5">
         <f t="shared" ref="H44:H47" si="30">H43</f>
         <v>22.27</v>
       </c>
@@ -3025,22 +3023,22 @@
         <f t="shared" si="27"/>
         <v>1000</v>
       </c>
-      <c r="D45" s="8">
+      <c r="D45" s="7">
         <f t="shared" si="28"/>
         <v>42</v>
       </c>
-      <c r="E45" s="8">
+      <c r="E45" s="7">
         <f t="shared" si="29"/>
         <v>45</v>
       </c>
       <c r="F45" s="2">
         <v>3.2300000000000002E-2</v>
       </c>
-      <c r="G45" s="9">
+      <c r="G45" s="8">
         <f t="shared" si="3"/>
         <v>1.2232415902140598E-2</v>
       </c>
-      <c r="H45" s="6">
+      <c r="H45" s="5">
         <f t="shared" si="30"/>
         <v>22.27</v>
       </c>
@@ -3056,22 +3054,22 @@
         <f t="shared" si="27"/>
         <v>1000</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D46" s="7">
         <f t="shared" si="28"/>
         <v>43</v>
       </c>
-      <c r="E46" s="8">
+      <c r="E46" s="7">
         <f t="shared" si="29"/>
         <v>45</v>
       </c>
       <c r="F46" s="2">
         <v>3.1600000000000003E-2</v>
       </c>
-      <c r="G46" s="9">
+      <c r="G46" s="8">
         <f t="shared" si="3"/>
         <v>2.1671826625386973E-2</v>
       </c>
-      <c r="H46" s="6">
+      <c r="H46" s="5">
         <f t="shared" si="30"/>
         <v>22.27</v>
       </c>
@@ -3087,22 +3085,22 @@
         <f t="shared" si="27"/>
         <v>1000</v>
       </c>
-      <c r="D47" s="8">
+      <c r="D47" s="7">
         <f t="shared" si="28"/>
         <v>44</v>
       </c>
-      <c r="E47" s="8">
+      <c r="E47" s="7">
         <f t="shared" si="29"/>
         <v>45</v>
       </c>
       <c r="F47" s="2">
         <v>3.1199999999999999E-2</v>
       </c>
-      <c r="G47" s="9">
+      <c r="G47" s="8">
         <f t="shared" si="3"/>
         <v>1.2658227848101408E-2</v>
       </c>
-      <c r="H47" s="6">
+      <c r="H47" s="5">
         <f t="shared" si="30"/>
         <v>22.27</v>
       </c>
@@ -3118,22 +3116,22 @@
         <f t="shared" ref="C48" si="31">C47</f>
         <v>1000</v>
       </c>
-      <c r="D48" s="8">
+      <c r="D48" s="7">
         <f t="shared" ref="D48" si="32">D47+1</f>
         <v>45</v>
       </c>
-      <c r="E48" s="8">
+      <c r="E48" s="7">
         <f t="shared" ref="E48" si="33">E47</f>
         <v>45</v>
       </c>
       <c r="F48" s="2">
         <v>3.1600000000000003E-2</v>
       </c>
-      <c r="G48" s="9">
+      <c r="G48" s="8">
         <f t="shared" si="3"/>
         <v>-1.2820512820512966E-2</v>
       </c>
-      <c r="H48" s="6">
+      <c r="H48" s="5">
         <f t="shared" ref="H48" si="34">H47</f>
         <v>22.27</v>
       </c>
@@ -3157,7 +3155,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3172,19 +3170,19 @@
     <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:10" ht="23" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3194,33 +3192,33 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -3230,19 +3228,23 @@
       <c r="C4" s="2">
         <v>1000</v>
       </c>
-      <c r="D4" s="11">
-        <v>1</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
         <v>30</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="6">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="5">
         <v>27.65</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J4" s="12">
+        <f>SUM(H4:H27)</f>
+        <v>663.59999999999968</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -3253,25 +3255,29 @@
         <f>C4</f>
         <v>1000</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="2">
         <f>D4+1</f>
         <v>2</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <f>E4</f>
         <v>30</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="9" t="str">
+      <c r="G5" s="8" t="str">
         <f>IF(F5&lt;&gt;"",(F4-F5)/F4,"")</f>
         <v/>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <f>H4</f>
         <v>27.65</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J5">
+        <f>J4*0.666666</f>
+        <v>442.39955759999975</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -3282,25 +3288,29 @@
         <f t="shared" ref="C6:C33" si="0">C5</f>
         <v>1000</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <f t="shared" ref="D6:D33" si="1">D5+1</f>
         <v>3</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <f t="shared" ref="E6:E11" si="2">E5</f>
         <v>30</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="9" t="str">
+      <c r="G6" s="8" t="str">
         <f t="shared" ref="G6:G33" si="3">IF(F6&lt;&gt;"",(F5-F6)/F5,"")</f>
         <v/>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <f t="shared" ref="H6:H33" si="4">H5</f>
         <v>27.65</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J6">
+        <f>J5/60</f>
+        <v>7.3733259599999963</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -3311,25 +3321,25 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="9" t="str">
+      <c r="G7" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -3340,25 +3350,25 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="9" t="str">
+      <c r="G8" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -3369,25 +3379,25 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="9" t="str">
+      <c r="G9" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -3398,25 +3408,25 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="9" t="str">
+      <c r="G10" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -3427,25 +3437,25 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="9" t="str">
+      <c r="G11" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -3456,25 +3466,25 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <f>E11</f>
         <v>30</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="9" t="str">
+      <c r="G12" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -3485,25 +3495,25 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <f t="shared" ref="E13:E33" si="5">E12</f>
         <v>30</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="9" t="str">
+      <c r="G13" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -3514,25 +3524,25 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="7">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="9" t="str">
+      <c r="G14" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -3543,25 +3553,25 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="7">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="9" t="str">
+      <c r="G15" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -3572,20 +3582,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F16" s="2"/>
-      <c r="G16" s="9" t="str">
+      <c r="G16" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -3601,20 +3611,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F17" s="2"/>
-      <c r="G17" s="9" t="str">
+      <c r="G17" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -3630,20 +3640,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F18" s="2"/>
-      <c r="G18" s="9" t="str">
+      <c r="G18" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -3659,20 +3669,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="7">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F19" s="2"/>
-      <c r="G19" s="9" t="str">
+      <c r="G19" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -3688,20 +3698,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="7">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="9" t="str">
+      <c r="G20" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -3717,20 +3727,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="7">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F21" s="2"/>
-      <c r="G21" s="9" t="str">
+      <c r="G21" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -3746,24 +3756,24 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="7">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F22" s="2"/>
-      <c r="G22" s="9" t="str">
+      <c r="G22" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
-      <c r="N22" s="12"/>
+      <c r="N22" s="9"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
@@ -3776,20 +3786,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="7">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F23" s="2"/>
-      <c r="G23" s="9" t="str">
+      <c r="G23" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -3805,20 +3815,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="7">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F24" s="2"/>
-      <c r="G24" s="9" t="str">
+      <c r="G24" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -3834,20 +3844,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="7">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F25" s="2"/>
-      <c r="G25" s="9" t="str">
+      <c r="G25" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -3863,20 +3873,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="7">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="9" t="str">
+      <c r="G26" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -3892,20 +3902,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="7">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F27" s="2"/>
-      <c r="G27" s="9" t="str">
+      <c r="G27" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H27" s="6">
+      <c r="H27" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -3921,20 +3931,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="7">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F28" s="2"/>
-      <c r="G28" s="9" t="str">
+      <c r="G28" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -3950,20 +3960,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="7">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F29" s="2"/>
-      <c r="G29" s="9" t="str">
+      <c r="G29" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -3979,20 +3989,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="7">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F30" s="2"/>
-      <c r="G30" s="9" t="str">
+      <c r="G30" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -4008,20 +4018,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="7">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F31" s="2"/>
-      <c r="G31" s="9" t="str">
+      <c r="G31" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H31" s="6">
+      <c r="H31" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -4037,20 +4047,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="7">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F32" s="2"/>
-      <c r="G32" s="9" t="str">
+      <c r="G32" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H32" s="6">
+      <c r="H32" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
@@ -4066,20 +4076,20 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="7">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="7">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="F33" s="2"/>
-      <c r="G33" s="9" t="str">
+      <c r="G33" s="8" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H33" s="6">
+      <c r="H33" s="5">
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>

</xml_diff>

<commit_message>
Adicionando as imagens em dataframes menores
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AriosvaldoBarros\Desktop\Projeto final - Aprendizado de Máquina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9401B79B-A3FC-4CE2-8BE7-9198C7C14E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0B164B-4D35-4D81-AE41-E11762B0D23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{1AF00C1C-39EC-4648-B1B0-894BAF27F7E3}"/>
+    <workbookView xWindow="28680" yWindow="-5910" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1AF00C1C-39EC-4648-B1B0-894BAF27F7E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
     <sheet name="segmentation_balloon_1000seg_45" sheetId="2" r:id="rId2"/>
     <sheet name="segmentation_phone_1000seg_30ep" sheetId="3" r:id="rId3"/>
+    <sheet name="segmentation_phone_666seg_20ep" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="29">
   <si>
     <t>Segmentação</t>
   </si>
@@ -114,6 +115,18 @@
   <si>
     <t>segmentation_balloon_1000seg_45epochs</t>
   </si>
+  <si>
+    <t>segmentation_phone_1000seg_30epochs</t>
+  </si>
+  <si>
+    <t>segmentation_phone_666seg_20epochs</t>
+  </si>
+  <si>
+    <t>Minutos totais</t>
+  </si>
+  <si>
+    <t>Horas totais</t>
+  </si>
 </sst>
 </file>
 
@@ -167,9 +180,8 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -208,7 +220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -234,14 +246,21 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1576,22 +1595,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -1691,10 +1710,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{001AA7BB-65BE-4D85-ACAE-CF2C205CDB85}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65:D66"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -1711,16 +1730,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -3136,9 +3155,31 @@
         <v>22.27</v>
       </c>
     </row>
+    <row r="50" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F50" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G50" s="9"/>
+      <c r="H50" s="5">
+        <f>SUM(H19:H48)</f>
+        <v>668.0999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="6:8" x14ac:dyDescent="0.35">
+      <c r="F51" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G51" s="9"/>
+      <c r="H51" s="5">
+        <f>H50/60</f>
+        <v>11.134999999999996</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3152,10 +3193,967 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18A583A-1AEC-4CDE-B092-9DC97F5C3BA1}">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F35" sqref="F35:H36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="23" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>30</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="5">
+        <v>27.65</v>
+      </c>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <f>C4</f>
+        <v>1000</v>
+      </c>
+      <c r="D5" s="2">
+        <f>D4+1</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="7">
+        <f>E4</f>
+        <v>30</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="8" t="str">
+        <f>IF(F5&lt;&gt;"",(F4-F5)/F4,"")</f>
+        <v/>
+      </c>
+      <c r="H5" s="5">
+        <f>H4</f>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" ref="C6:C33" si="0">C5</f>
+        <v>1000</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" ref="D6:D33" si="1">D5+1</f>
+        <v>3</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" ref="E6:E11" si="2">E5</f>
+        <v>30</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="8" t="str">
+        <f t="shared" ref="G6:G33" si="3">IF(F6&lt;&gt;"",(F5-F6)/F5,"")</f>
+        <v/>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" ref="H6:H33" si="4">H5</f>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="E12" s="7">
+        <f>E11</f>
+        <v>30</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" ref="E13:E33" si="5">E12</f>
+        <v>30</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H16" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H17" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H18" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="E19" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H19" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H20" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="E22" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H22" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+      <c r="N22" s="12"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="E23" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="E24" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H24" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="E25" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H25" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="E26" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H26" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D27" s="7">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="E27" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H27" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="E28" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H28" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="E29" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H29" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="E30" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H30" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="E31" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H31" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="E32" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H32" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="E33" s="7">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H33" s="5">
+        <f t="shared" si="4"/>
+        <v>27.65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F35" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G35" s="9"/>
+      <c r="H35" s="5">
+        <f>SUM(H4:H33)</f>
+        <v>829.49999999999955</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F36" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="9"/>
+      <c r="H36" s="5">
+        <f>H35/60</f>
+        <v>13.824999999999992</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <ignoredErrors>
+    <ignoredError sqref="D5:D33" formula="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC1740D-DFC2-4FD1-83B3-6C39DE1EB110}">
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3166,23 +4164,23 @@
     <col min="4" max="4" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.36328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3192,7 +4190,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -3218,7 +4216,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -3236,15 +4234,9 @@
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="5">
-        <v>27.65</v>
-      </c>
-      <c r="J4" s="12">
-        <f>SUM(H4:H27)</f>
-        <v>663.59999999999968</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -3268,16 +4260,9 @@
         <f>IF(F5&lt;&gt;"",(F4-F5)/F4,"")</f>
         <v/>
       </c>
-      <c r="H5" s="5">
-        <f>H4</f>
-        <v>27.65</v>
-      </c>
-      <c r="J5">
-        <f>J4*0.666666</f>
-        <v>442.39955759999975</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -3285,11 +4270,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" ref="C6:C33" si="0">C5</f>
+        <f t="shared" ref="C6:C23" si="0">C5</f>
         <v>1000</v>
       </c>
       <c r="D6" s="7">
-        <f t="shared" ref="D6:D33" si="1">D5+1</f>
+        <f t="shared" ref="D6:D23" si="1">D5+1</f>
         <v>3</v>
       </c>
       <c r="E6" s="7">
@@ -3298,19 +4283,12 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="8" t="str">
-        <f t="shared" ref="G6:G33" si="3">IF(F6&lt;&gt;"",(F5-F6)/F5,"")</f>
+        <f t="shared" ref="G6:G23" si="3">IF(F6&lt;&gt;"",(F5-F6)/F5,"")</f>
         <v/>
       </c>
-      <c r="H6" s="5">
-        <f t="shared" ref="H6:H33" si="4">H5</f>
-        <v>27.65</v>
-      </c>
-      <c r="J6">
-        <f>J5/60</f>
-        <v>7.3733259599999963</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -3334,12 +4312,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H7" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -3363,12 +4338,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H8" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -3392,12 +4364,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H9" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -3421,12 +4390,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H10" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -3450,12 +4416,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H11" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -3479,12 +4442,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H12" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -3500,7 +4460,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="7">
-        <f t="shared" ref="E13:E33" si="5">E12</f>
+        <f t="shared" ref="E13:E23" si="4">E12</f>
         <v>30</v>
       </c>
       <c r="F13" s="2"/>
@@ -3508,12 +4468,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H13" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -3529,7 +4486,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="F14" s="2"/>
@@ -3537,12 +4494,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H14" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -3558,7 +4512,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="F15" s="2"/>
@@ -3566,12 +4520,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H15" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -3587,7 +4538,7 @@
         <v>13</v>
       </c>
       <c r="E16" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="F16" s="2"/>
@@ -3595,12 +4546,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H16" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -3616,7 +4564,7 @@
         <v>14</v>
       </c>
       <c r="E17" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="F17" s="2"/>
@@ -3624,12 +4572,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H17" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -3645,7 +4590,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="F18" s="2"/>
@@ -3653,12 +4598,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H18" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
@@ -3674,7 +4616,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="F19" s="2"/>
@@ -3682,12 +4624,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H19" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
@@ -3703,7 +4642,7 @@
         <v>17</v>
       </c>
       <c r="E20" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="F20" s="2"/>
@@ -3711,12 +4650,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H20" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
@@ -3732,7 +4668,7 @@
         <v>18</v>
       </c>
       <c r="E21" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="F21" s="2"/>
@@ -3740,12 +4676,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H21" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -3761,7 +4694,7 @@
         <v>19</v>
       </c>
       <c r="E22" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="F22" s="2"/>
@@ -3769,13 +4702,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H22" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-      <c r="N22" s="9"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -3791,7 +4720,7 @@
         <v>20</v>
       </c>
       <c r="E23" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="F23" s="2"/>
@@ -3799,308 +4728,37 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H23" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="2">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="D24" s="7">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="E24" s="7">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H24" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="2">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="D25" s="7">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="E25" s="7">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F25" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="9"/>
       <c r="H25" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="2">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="D26" s="7">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="E26" s="7">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H26" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="D27" s="7">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="E27" s="7">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H27" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="2">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="D28" s="7">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="E28" s="7">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H28" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="2">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="D29" s="7">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="E29" s="7">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H29" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="2">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="D30" s="7">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="E30" s="7">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="F30" s="2"/>
-      <c r="G30" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H30" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="D31" s="7">
-        <f t="shared" si="1"/>
+        <f>SUM(H4:H23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F26" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="7">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H31" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="2">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="D32" s="7">
-        <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="E32" s="7">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H32" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="2">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="D33" s="7">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="E33" s="7">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H33" s="5">
-        <f t="shared" si="4"/>
-        <v>27.65</v>
+      <c r="G26" s="9"/>
+      <c r="H26" s="13">
+        <f>H25/60</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <ignoredErrors>
-    <ignoredError sqref="D5:D33" formula="1"/>
+    <ignoredError sqref="D5:D23" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionando mais dataframes de imagens
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AriosvaldoBarros\Desktop\Projeto final - Aprendizado de Máquina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0B164B-4D35-4D81-AE41-E11762B0D23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC48B327-550A-46F6-ACCA-3415062085BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-5910" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1AF00C1C-39EC-4648-B1B0-894BAF27F7E3}"/>
   </bookViews>
@@ -135,7 +135,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +183,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -220,7 +228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -246,12 +254,6 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -261,6 +263,13 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1595,22 +1604,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -1730,16 +1739,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -3156,20 +3165,20 @@
       </c>
     </row>
     <row r="50" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F50" s="9" t="s">
+      <c r="F50" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G50" s="9"/>
+      <c r="G50" s="12"/>
       <c r="H50" s="5">
         <f>SUM(H19:H48)</f>
         <v>668.0999999999998</v>
       </c>
     </row>
     <row r="51" spans="6:8" x14ac:dyDescent="0.35">
-      <c r="F51" s="9" t="s">
+      <c r="F51" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G51" s="9"/>
+      <c r="G51" s="12"/>
       <c r="H51" s="5">
         <f>H50/60</f>
         <v>11.134999999999996</v>
@@ -3196,7 +3205,7 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35:H36"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -3213,16 +3222,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -3271,7 +3280,7 @@
       <c r="H4" s="5">
         <v>27.65</v>
       </c>
-      <c r="J4" s="11"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -3794,7 +3803,7 @@
         <f t="shared" si="4"/>
         <v>27.65</v>
       </c>
-      <c r="N22" s="12"/>
+      <c r="N22" s="10"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
@@ -4116,20 +4125,20 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F35" s="9" t="s">
+      <c r="F35" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G35" s="9"/>
+      <c r="G35" s="12"/>
       <c r="H35" s="5">
         <f>SUM(H4:H33)</f>
         <v>829.49999999999955</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F36" s="9" t="s">
+      <c r="F36" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G36" s="9"/>
+      <c r="G36" s="12"/>
       <c r="H36" s="5">
         <f>H35/60</f>
         <v>13.824999999999992</v>
@@ -4150,10 +4159,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC1740D-DFC2-4FD1-83B3-6C39DE1EB110}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4169,16 +4178,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -4234,7 +4243,9 @@
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="5"/>
+      <c r="H4" s="5">
+        <v>18.876999999999999</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -4260,7 +4271,9 @@
         <f>IF(F5&lt;&gt;"",(F4-F5)/F4,"")</f>
         <v/>
       </c>
-      <c r="H5" s="5"/>
+      <c r="H5" s="5">
+        <v>18.876999999999999</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -4286,7 +4299,9 @@
         <f t="shared" ref="G6:G23" si="3">IF(F6&lt;&gt;"",(F5-F6)/F5,"")</f>
         <v/>
       </c>
-      <c r="H6" s="5"/>
+      <c r="H6" s="5">
+        <v>18.876999999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
@@ -4312,7 +4327,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H7" s="5"/>
+      <c r="H7" s="5">
+        <v>18.876999999999999</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -4338,7 +4355,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H8" s="5"/>
+      <c r="H8" s="5">
+        <v>18.876999999999999</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
@@ -4364,7 +4383,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H9" s="5"/>
+      <c r="H9" s="5">
+        <v>18.876999999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
@@ -4390,7 +4411,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H10" s="5"/>
+      <c r="H10" s="5">
+        <v>18.876999999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
@@ -4416,7 +4439,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H11" s="5"/>
+      <c r="H11" s="5">
+        <v>18.876999999999999</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
@@ -4442,7 +4467,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H12" s="5"/>
+      <c r="H12" s="5">
+        <v>18.876999999999999</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
@@ -4468,7 +4495,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H13" s="5"/>
+      <c r="H13" s="5">
+        <v>18.876999999999999</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
@@ -4494,7 +4523,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="5">
+        <v>18.876999999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
@@ -4520,7 +4551,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H15" s="5"/>
+      <c r="H15" s="5">
+        <v>18.876999999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
@@ -4546,9 +4579,11 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H16" s="5">
+        <v>18.876999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -4572,9 +4607,11 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H17" s="5">
+        <v>18.876999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -4598,9 +4635,11 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H18" s="5">
+        <v>18.876999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
@@ -4624,9 +4663,12 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H19" s="5">
+        <v>18.876999999999999</v>
+      </c>
+      <c r="K19" s="14"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
@@ -4650,9 +4692,11 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H20" s="5">
+        <v>18.876999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
@@ -4676,9 +4720,11 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H21" s="5">
+        <v>18.876999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -4702,9 +4748,11 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H22" s="5">
+        <v>18.876999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -4728,26 +4776,28 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F25" s="9" t="s">
+      <c r="H23" s="5">
+        <v>18.876999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F25" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="9"/>
+      <c r="G25" s="12"/>
       <c r="H25" s="5">
         <f>SUM(H4:H23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F26" s="9" t="s">
+        <v>377.54000000000008</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F26" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="13">
+      <c r="G26" s="12"/>
+      <c r="H26" s="11">
         <f>H25/60</f>
-        <v>0</v>
+        <v>6.2923333333333344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>